<commit_message>
bugfix: fixed a misplacement in xls file for A2b cards + added Promo-A from A2b cards
</commit_message>
<xml_diff>
--- a/scripts/correspondences.xlsx
+++ b/scripts/correspondences.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathy\Desktop\Projets\tcg-pocket-collection-tracker\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{020CCDED-2D8A-490F-A3EC-F012F4456B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB590906-B3AA-430D-9241-EE1334D6E033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="621">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="647">
   <si>
     <t>cTR_10</t>
   </si>
@@ -1660,9 +1660,6 @@
     <t>cPK_20_005350_00</t>
   </si>
   <si>
-    <t>cPK_10_005810_00</t>
-  </si>
-  <si>
     <t>cPK_20_005760_00</t>
   </si>
   <si>
@@ -1892,6 +1889,87 @@
   </si>
   <si>
     <t>[Gold] - Poké Ball</t>
+  </si>
+  <si>
+    <t>cPK_20_005260_00</t>
+  </si>
+  <si>
+    <t>cPK_90_001290_00</t>
+  </si>
+  <si>
+    <t>cPK_90_005090_00</t>
+  </si>
+  <si>
+    <t>cPK_90_005080_00</t>
+  </si>
+  <si>
+    <t>cPK_90_005000_00</t>
+  </si>
+  <si>
+    <t>cPK_90_005010_00</t>
+  </si>
+  <si>
+    <t>cPK_90_005020_00</t>
+  </si>
+  <si>
+    <t>cPK_90_005040_00</t>
+  </si>
+  <si>
+    <t>cPK_90_005060_00</t>
+  </si>
+  <si>
+    <t>cPK_90_005070_00</t>
+  </si>
+  <si>
+    <t>cPK_90_005030_00</t>
+  </si>
+  <si>
+    <t>[Shiny] - Mewtwo ex</t>
+  </si>
+  <si>
+    <t>[Shiny] - Cyclizar</t>
+  </si>
+  <si>
+    <t>[Full Art] - Sprigatito</t>
+  </si>
+  <si>
+    <t>Floatzel</t>
+  </si>
+  <si>
+    <t>[Full Art] - Pawmot</t>
+  </si>
+  <si>
+    <t>Ekans</t>
+  </si>
+  <si>
+    <t>P-A_050</t>
+  </si>
+  <si>
+    <t>P-A_051</t>
+  </si>
+  <si>
+    <t>P-A_052</t>
+  </si>
+  <si>
+    <t>P-A_053</t>
+  </si>
+  <si>
+    <t>P-A_054</t>
+  </si>
+  <si>
+    <t>P-A_055</t>
+  </si>
+  <si>
+    <t>P-A_056</t>
+  </si>
+  <si>
+    <t>P-A_057</t>
+  </si>
+  <si>
+    <t>P-A_058</t>
+  </si>
+  <si>
+    <t>P-A_059</t>
   </si>
 </sst>
 </file>
@@ -2237,8 +2315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3107,7 +3185,7 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3513,7 +3591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8371A10B-6886-4A14-BFE6-3986A0B1B338}">
   <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
@@ -4161,8 +4239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5343CA1F-1CEA-4E4E-A2BE-AAAC7099C72D}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4488,10 +4566,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01A8222D-5E44-433B-93F3-4227EF9A3A72}">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4602,10 +4680,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B10" t="s">
-        <v>543</v>
+        <v>620</v>
       </c>
       <c r="C10" t="s">
         <v>45</v>
@@ -4613,7 +4691,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B11" t="s">
         <v>542</v>
@@ -4624,7 +4702,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B12" t="s">
         <v>541</v>
@@ -4635,7 +4713,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B13" t="s">
         <v>540</v>
@@ -4646,7 +4724,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B14" t="s">
         <v>539</v>
@@ -4657,10 +4735,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B15" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C15" t="s">
         <v>54</v>
@@ -4668,10 +4746,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B16" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C16" t="s">
         <v>116</v>
@@ -4682,7 +4760,7 @@
         <v>273</v>
       </c>
       <c r="B17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C17" t="s">
         <v>118</v>
@@ -4690,10 +4768,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B18" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C18" t="s">
         <v>119</v>
@@ -4704,7 +4782,7 @@
         <v>279</v>
       </c>
       <c r="B19" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C19" t="s">
         <v>120</v>
@@ -4712,10 +4790,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B20" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C20" t="s">
         <v>121</v>
@@ -4723,21 +4801,21 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B21" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C21" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B22" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C22" t="s">
         <v>374</v>
@@ -4745,10 +4823,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B23" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C23" t="s">
         <v>375</v>
@@ -4756,10 +4834,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B24" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C24" t="s">
         <v>376</v>
@@ -4767,233 +4845,343 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>286</v>
+        <v>619</v>
       </c>
       <c r="B25" t="s">
-        <v>73</v>
+        <v>560</v>
       </c>
       <c r="C25" t="s">
-        <v>117</v>
+        <v>587</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>599</v>
+        <v>286</v>
       </c>
       <c r="B26" t="s">
-        <v>559</v>
+        <v>73</v>
       </c>
       <c r="C26" t="s">
-        <v>379</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="B27" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C27" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="B28" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="C28" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="B29" t="s">
         <v>557</v>
       </c>
       <c r="C29" t="s">
-        <v>94</v>
+        <v>381</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>601</v>
+      </c>
+      <c r="B30" t="s">
         <v>556</v>
       </c>
-      <c r="B30" t="s">
-        <v>555</v>
-      </c>
       <c r="C30" t="s">
-        <v>386</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>606</v>
+        <v>555</v>
       </c>
       <c r="B31" t="s">
-        <v>562</v>
+        <v>554</v>
       </c>
       <c r="C31" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="B32" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="C32" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B33" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="C33" t="s">
-        <v>576</v>
+        <v>389</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="B34" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="C34" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="B35" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="C35" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="B36" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="C36" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="B37" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C37" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="B38" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C38" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="B39" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="C39" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="B40" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="C40" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="B41" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="C41" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B42" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="C42" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="B43" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="C43" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B44" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C44" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="B45" t="s">
-        <v>561</v>
+        <v>574</v>
       </c>
       <c r="C45" t="s">
-        <v>588</v>
+        <v>586</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>631</v>
+      </c>
+      <c r="B46" t="s">
+        <v>621</v>
+      </c>
+      <c r="C46" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>632</v>
+      </c>
+      <c r="B47" t="s">
+        <v>622</v>
+      </c>
+      <c r="C47" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>633</v>
+      </c>
+      <c r="B48" t="s">
+        <v>623</v>
+      </c>
+      <c r="C48" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>634</v>
+      </c>
+      <c r="B49" t="s">
+        <v>624</v>
+      </c>
+      <c r="C49" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>635</v>
+      </c>
+      <c r="B50" t="s">
+        <v>625</v>
+      </c>
+      <c r="C50" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>525</v>
+      </c>
+      <c r="B51" t="s">
+        <v>626</v>
+      </c>
+      <c r="C51" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>636</v>
+      </c>
+      <c r="B52" t="s">
+        <v>630</v>
+      </c>
+      <c r="C52" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>532</v>
+      </c>
+      <c r="B53" t="s">
+        <v>627</v>
+      </c>
+      <c r="C53" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>533</v>
+      </c>
+      <c r="B54" t="s">
+        <v>628</v>
+      </c>
+      <c r="C54" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>529</v>
+      </c>
+      <c r="B55" t="s">
+        <v>629</v>
+      </c>
+      <c r="C55" t="s">
+        <v>646</v>
       </c>
     </row>
   </sheetData>

</xml_diff>